<commit_message>
Preparing for vignette release
</commit_message>
<xml_diff>
--- a/inst/extdata/martysweight.xlsx
+++ b/inst/extdata/martysweight.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mrkmartongmailcom.sharepoint.com/sites/-/Shared Documents/General/Stats_R/R/Martysweight/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1454" documentId="13_ncr:1_{F102E521-F1A2-407A-A6A3-36972B24CEEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{745A26F0-44F6-4BA8-934D-7E3F0D636B70}"/>
+  <xr:revisionPtr revIDLastSave="1484" documentId="13_ncr:1_{F102E521-F1A2-407A-A6A3-36972B24CEEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FFC9EF6D-6C1D-4F1A-990E-DDF6876C1B63}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FC665D15-152F-4F01-8A80-E2816C212E79}"/>
   </bookViews>
@@ -470,11 +470,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39223600-1D15-461E-B723-4E7F83AA1860}">
-  <dimension ref="A1:G2181"/>
+  <dimension ref="A1:G2186"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2160" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2182" sqref="F2182"/>
+      <selection pane="bottomLeft" activeCell="F2187" sqref="F2187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37048,6 +37048,106 @@
         <v>23</v>
       </c>
       <c r="F2181" s="4">
+        <v>86.1</v>
+      </c>
+    </row>
+    <row r="2182" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2182" s="1">
+        <v>45269</v>
+      </c>
+      <c r="B2182">
+        <v>10</v>
+      </c>
+      <c r="C2182">
+        <v>10</v>
+      </c>
+      <c r="D2182">
+        <v>0</v>
+      </c>
+      <c r="E2182">
+        <v>10</v>
+      </c>
+      <c r="F2182" s="4">
+        <v>86.1</v>
+      </c>
+    </row>
+    <row r="2183" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2183" s="1">
+        <v>45270</v>
+      </c>
+      <c r="B2183">
+        <v>21</v>
+      </c>
+      <c r="C2183">
+        <v>25</v>
+      </c>
+      <c r="D2183">
+        <v>1</v>
+      </c>
+      <c r="E2183">
+        <v>0</v>
+      </c>
+      <c r="F2183" s="4">
+        <v>86.7</v>
+      </c>
+    </row>
+    <row r="2184" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2184" s="1">
+        <v>45271</v>
+      </c>
+      <c r="B2184">
+        <v>18</v>
+      </c>
+      <c r="C2184">
+        <v>35</v>
+      </c>
+      <c r="D2184">
+        <v>0</v>
+      </c>
+      <c r="E2184">
+        <v>10</v>
+      </c>
+      <c r="F2184" s="4">
+        <v>86.2</v>
+      </c>
+    </row>
+    <row r="2185" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2185" s="1">
+        <v>45272</v>
+      </c>
+      <c r="B2185">
+        <v>8</v>
+      </c>
+      <c r="C2185">
+        <v>10</v>
+      </c>
+      <c r="D2185">
+        <v>13</v>
+      </c>
+      <c r="E2185">
+        <v>45</v>
+      </c>
+      <c r="F2185" s="4">
+        <v>85.8</v>
+      </c>
+    </row>
+    <row r="2186" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2186" s="1">
+        <v>45273</v>
+      </c>
+      <c r="B2186">
+        <v>12</v>
+      </c>
+      <c r="C2186">
+        <v>25</v>
+      </c>
+      <c r="D2186">
+        <v>4</v>
+      </c>
+      <c r="E2186">
+        <v>0</v>
+      </c>
+      <c r="F2186" s="4">
         <v>86.1</v>
       </c>
     </row>
@@ -37062,6 +37162,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a95d4ba5-ac50-4ccb-8f38-68d250b34105" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3073c576-dbcc-4dca-a8e5-ccf7a0688d93">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F0ADBC3A86B10A4085B52F181C274AA0" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8197e89490dc663f80df425c475dfb63">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3073c576-dbcc-4dca-a8e5-ccf7a0688d93" xmlns:ns3="a95d4ba5-ac50-4ccb-8f38-68d250b34105" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="57d494f76f6743b951aebebbdbb44cb6" ns2:_="" ns3:_="">
     <xsd:import namespace="3073c576-dbcc-4dca-a8e5-ccf7a0688d93"/>
@@ -37276,27 +37396,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a95d4ba5-ac50-4ccb-8f38-68d250b34105" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3073c576-dbcc-4dca-a8e5-ccf7a0688d93">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4A0FCBE-B2C0-4543-8CC5-CB84272EA876}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60E55020-46B3-40ED-BFB8-4929986AA94A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a95d4ba5-ac50-4ccb-8f38-68d250b34105"/>
+    <ds:schemaRef ds:uri="3073c576-dbcc-4dca-a8e5-ccf7a0688d93"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37357D95-8B77-409A-BAF8-E831BCA8A58F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -37313,23 +37432,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60E55020-46B3-40ED-BFB8-4929986AA94A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a95d4ba5-ac50-4ccb-8f38-68d250b34105"/>
-    <ds:schemaRef ds:uri="3073c576-dbcc-4dca-a8e5-ccf7a0688d93"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4A0FCBE-B2C0-4543-8CC5-CB84272EA876}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>